<commit_message>
Fixed a few mistakes in datasets and rerun the whole code
</commit_message>
<xml_diff>
--- a/Datasets/Reduced_version-normalized.xlsx
+++ b/Datasets/Reduced_version-normalized.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="64">
   <si>
     <t>Authors</t>
   </si>
@@ -124,7 +124,7 @@
     <t>Total_final_organic_C_mM</t>
   </si>
   <si>
-    <t>C_conversion_ratio</t>
+    <t>C_ratio</t>
   </si>
   <si>
     <t>Huang 2016 SR</t>
@@ -563,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL159"/>
+  <dimension ref="A1:AL158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3650,7 +3650,7 @@
         <v>0.7131147540983607</v>
       </c>
       <c r="W27">
-        <v>0.1107011070110701</v>
+        <v>0.05535055350553506</v>
       </c>
       <c r="X27">
         <v>1</v>
@@ -3766,7 +3766,7 @@
         <v>0.3934426229508197</v>
       </c>
       <c r="W28">
-        <v>0.1107011070110701</v>
+        <v>0.05535055350553506</v>
       </c>
       <c r="X28">
         <v>1</v>
@@ -17629,13 +17629,13 @@
         <v>1</v>
       </c>
       <c r="D148">
-        <v>0.5768421052631579</v>
+        <v>0.4336842105263158</v>
       </c>
       <c r="E148">
         <v>0.09974278365247213</v>
       </c>
       <c r="F148">
-        <v>0.5965130006341772</v>
+        <v>0.1066978877018391</v>
       </c>
       <c r="G148">
         <v>1</v>
@@ -17671,7 +17671,7 @@
         <v>0</v>
       </c>
       <c r="R148">
-        <v>0.00405618568316683</v>
+        <v>-1</v>
       </c>
       <c r="S148">
         <v>0.1766666666666667</v>
@@ -17683,10 +17683,10 @@
         <v>-1</v>
       </c>
       <c r="V148">
-        <v>0.707377049180328</v>
+        <v>0.5204918032786885</v>
       </c>
       <c r="W148">
-        <v>1.845018450184502e-05</v>
+        <v>0.3690036900369004</v>
       </c>
       <c r="X148">
         <v>0</v>
@@ -17719,19 +17719,19 @@
         <v>0</v>
       </c>
       <c r="AH148">
-        <v>0.006392156862745098</v>
+        <v>0.002196078431372549</v>
       </c>
       <c r="AI148">
-        <v>0.0006738831615120274</v>
+        <v>0.0003024054982817869</v>
       </c>
       <c r="AJ148">
         <v>0</v>
       </c>
       <c r="AK148">
-        <v>0.003029628096402822</v>
+        <v>0.002966599517810966</v>
       </c>
       <c r="AL148">
-        <v>3.922</v>
+        <v>8.800000000000001e-05</v>
       </c>
     </row>
     <row r="149" spans="1:38">
@@ -17739,22 +17739,22 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C149">
         <v>1</v>
       </c>
       <c r="D149">
-        <v>0.4336842105263158</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="E149">
         <v>0.09974278365247213</v>
       </c>
       <c r="F149">
-        <v>0.1066978877018391</v>
+        <v>0.6556905214888531</v>
       </c>
       <c r="G149">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H149">
         <v>0</v>
@@ -17763,7 +17763,7 @@
         <v>0</v>
       </c>
       <c r="J149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K149">
         <v>0</v>
@@ -17784,31 +17784,31 @@
         <v>0</v>
       </c>
       <c r="Q149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R149">
-        <v>-1</v>
+        <v>0.004406720248378779</v>
       </c>
       <c r="S149">
-        <v>0.1766666666666667</v>
+        <v>1</v>
       </c>
       <c r="T149">
-        <v>0.07066666666666667</v>
+        <v>1</v>
       </c>
       <c r="U149">
-        <v>-1</v>
+        <v>0.5779569892473119</v>
       </c>
       <c r="V149">
-        <v>0.5204918032786885</v>
+        <v>0.7377049180327869</v>
       </c>
       <c r="W149">
-        <v>0.3690036900369004</v>
+        <v>1.845018450184502e-05</v>
       </c>
       <c r="X149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z149">
         <v>0</v>
@@ -17817,7 +17817,7 @@
         <v>0</v>
       </c>
       <c r="AB149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC149">
         <v>0</v>
@@ -17826,7 +17826,7 @@
         <v>1</v>
       </c>
       <c r="AE149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF149">
         <v>0</v>
@@ -17835,19 +17835,19 @@
         <v>0</v>
       </c>
       <c r="AH149">
-        <v>0.002196078431372549</v>
+        <v>0.01509803921568627</v>
       </c>
       <c r="AI149">
-        <v>0.0003024054982817869</v>
+        <v>-1</v>
       </c>
       <c r="AJ149">
         <v>0</v>
       </c>
       <c r="AK149">
-        <v>0.002966599517810966</v>
+        <v>0</v>
       </c>
       <c r="AL149">
-        <v>8.800000000000001e-05</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="150" spans="1:38">
@@ -17855,19 +17855,19 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C150">
         <v>1</v>
       </c>
       <c r="D150">
-        <v>0.5789473684210527</v>
+        <v>0.4757894736842105</v>
       </c>
       <c r="E150">
-        <v>0.09974278365247213</v>
+        <v>0.04829951414689911</v>
       </c>
       <c r="F150">
-        <v>0.6556905214888531</v>
+        <v>0.003658715059271184</v>
       </c>
       <c r="G150">
         <v>0</v>
@@ -17876,10 +17876,10 @@
         <v>0</v>
       </c>
       <c r="I150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K150">
         <v>0</v>
@@ -17888,10 +17888,10 @@
         <v>0</v>
       </c>
       <c r="M150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O150">
         <v>0</v>
@@ -17900,31 +17900,31 @@
         <v>0</v>
       </c>
       <c r="Q150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R150">
-        <v>0.004406720248378779</v>
+        <v>0.06106812889656727</v>
       </c>
       <c r="S150">
-        <v>1</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="T150">
-        <v>1</v>
+        <v>0.02466666666666667</v>
       </c>
       <c r="U150">
-        <v>0.5779569892473119</v>
+        <v>0.05376344086021505</v>
       </c>
       <c r="V150">
-        <v>0.7377049180327869</v>
+        <v>-1</v>
       </c>
       <c r="W150">
-        <v>1.845018450184502e-05</v>
+        <v>0</v>
       </c>
       <c r="X150">
         <v>1</v>
       </c>
       <c r="Y150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z150">
         <v>0</v>
@@ -17933,10 +17933,10 @@
         <v>0</v>
       </c>
       <c r="AB150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD150">
         <v>1</v>
@@ -17951,16 +17951,16 @@
         <v>0</v>
       </c>
       <c r="AH150">
-        <v>0.01509803921568627</v>
+        <v>0.6862745098039216</v>
       </c>
       <c r="AI150">
-        <v>-1</v>
+        <v>0.000859106529209622</v>
       </c>
       <c r="AJ150">
-        <v>0</v>
+        <v>0.002925287674667428</v>
       </c>
       <c r="AK150">
-        <v>0</v>
+        <v>0.003070966914369173</v>
       </c>
       <c r="AL150">
         <v>-1</v>
@@ -17974,16 +17974,16 @@
         <v>63</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D151">
-        <v>0.4757894736842105</v>
+        <v>0.4842105263157895</v>
       </c>
       <c r="E151">
         <v>0.04829951414689911</v>
       </c>
       <c r="F151">
-        <v>0.003658715059271184</v>
+        <v>0.004585589540953217</v>
       </c>
       <c r="G151">
         <v>0</v>
@@ -18019,7 +18019,7 @@
         <v>0</v>
       </c>
       <c r="R151">
-        <v>0.06106812889656727</v>
+        <v>0.07669195523172839</v>
       </c>
       <c r="S151">
         <v>0.2466666666666667</v>
@@ -18067,16 +18067,16 @@
         <v>0</v>
       </c>
       <c r="AH151">
-        <v>0.6862745098039216</v>
+        <v>0.7450980392156863</v>
       </c>
       <c r="AI151">
-        <v>0.000859106529209622</v>
+        <v>0.001151202749140893</v>
       </c>
       <c r="AJ151">
-        <v>0.002925287674667428</v>
+        <v>0.002920914611569958</v>
       </c>
       <c r="AK151">
-        <v>0.003070966914369173</v>
+        <v>0.003116153915672308</v>
       </c>
       <c r="AL151">
         <v>-1</v>
@@ -18090,7 +18090,7 @@
         <v>63</v>
       </c>
       <c r="C152">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D152">
         <v>0.4842105263157895</v>
@@ -18099,7 +18099,7 @@
         <v>0.04829951414689911</v>
       </c>
       <c r="F152">
-        <v>0.004585589540953217</v>
+        <v>0.00331723498707254</v>
       </c>
       <c r="G152">
         <v>0</v>
@@ -18135,7 +18135,7 @@
         <v>0</v>
       </c>
       <c r="R152">
-        <v>0.07669195523172839</v>
+        <v>0.05234793404769861</v>
       </c>
       <c r="S152">
         <v>0.2466666666666667</v>
@@ -18144,13 +18144,13 @@
         <v>0.02466666666666667</v>
       </c>
       <c r="U152">
-        <v>0.05376344086021505</v>
+        <v>0.08064516129032259</v>
       </c>
       <c r="V152">
         <v>-1</v>
       </c>
       <c r="W152">
-        <v>0</v>
+        <v>0.1476014760147601</v>
       </c>
       <c r="X152">
         <v>1</v>
@@ -18183,19 +18183,19 @@
         <v>0</v>
       </c>
       <c r="AH152">
-        <v>0.7450980392156863</v>
+        <v>0.6274509803921569</v>
       </c>
       <c r="AI152">
-        <v>0.001151202749140893</v>
+        <v>0.01890034364261169</v>
       </c>
       <c r="AJ152">
-        <v>0.002920914611569958</v>
+        <v>0.02492645965557754</v>
       </c>
       <c r="AK152">
-        <v>0.003116153915672308</v>
+        <v>0.02813255242420972</v>
       </c>
       <c r="AL152">
-        <v>-1</v>
+        <v>0.108125</v>
       </c>
     </row>
     <row r="153" spans="1:38">
@@ -18206,16 +18206,16 @@
         <v>63</v>
       </c>
       <c r="C153">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D153">
-        <v>0.4842105263157895</v>
+        <v>0.48</v>
       </c>
       <c r="E153">
         <v>0.04829951414689911</v>
       </c>
       <c r="F153">
-        <v>0.00331723498707254</v>
+        <v>0.0139031172252305</v>
       </c>
       <c r="G153">
         <v>0</v>
@@ -18251,7 +18251,7 @@
         <v>0</v>
       </c>
       <c r="R153">
-        <v>0.05234793404769861</v>
+        <v>0.04749108587779463</v>
       </c>
       <c r="S153">
         <v>0.2466666666666667</v>
@@ -18260,10 +18260,10 @@
         <v>0.02466666666666667</v>
       </c>
       <c r="U153">
-        <v>0.08064516129032259</v>
+        <v>0</v>
       </c>
       <c r="V153">
-        <v>-1</v>
+        <v>0.3278688524590164</v>
       </c>
       <c r="W153">
         <v>0.1476014760147601</v>
@@ -18302,16 +18302,16 @@
         <v>0.6274509803921569</v>
       </c>
       <c r="AI153">
-        <v>0.01890034364261169</v>
+        <v>0.03951890034364261</v>
       </c>
       <c r="AJ153">
-        <v>0.02492645965557754</v>
+        <v>0.01956216892268132</v>
       </c>
       <c r="AK153">
-        <v>0.02813255242420972</v>
+        <v>0.02626676656395126</v>
       </c>
       <c r="AL153">
-        <v>0.108125</v>
+        <v>0.100125</v>
       </c>
     </row>
     <row r="154" spans="1:38">
@@ -18322,16 +18322,16 @@
         <v>63</v>
       </c>
       <c r="C154">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D154">
-        <v>0.48</v>
+        <v>0.4884210526315789</v>
       </c>
       <c r="E154">
-        <v>0.04829951414689911</v>
+        <v>0.09974278365247213</v>
       </c>
       <c r="F154">
-        <v>0.0139031172252305</v>
+        <v>0.01175667105712474</v>
       </c>
       <c r="G154">
         <v>0</v>
@@ -18367,7 +18367,7 @@
         <v>0</v>
       </c>
       <c r="R154">
-        <v>0.04749108587779463</v>
+        <v>0.04095124375016729</v>
       </c>
       <c r="S154">
         <v>0.2466666666666667</v>
@@ -18376,10 +18376,10 @@
         <v>0.02466666666666667</v>
       </c>
       <c r="U154">
-        <v>0</v>
+        <v>0.1747311827956989</v>
       </c>
       <c r="V154">
-        <v>0.3278688524590164</v>
+        <v>-1</v>
       </c>
       <c r="W154">
         <v>0.1476014760147601</v>
@@ -18415,19 +18415,19 @@
         <v>0</v>
       </c>
       <c r="AH154">
-        <v>0.6274509803921569</v>
+        <v>0.7254901960784313</v>
       </c>
       <c r="AI154">
-        <v>0.03951890034364261</v>
+        <v>0.02920962199312714</v>
       </c>
       <c r="AJ154">
-        <v>0.01956216892268132</v>
+        <v>0.02145716293158488</v>
       </c>
       <c r="AK154">
-        <v>0.02626676656395126</v>
+        <v>0.02641253108428395</v>
       </c>
       <c r="AL154">
-        <v>0.100125</v>
+        <v>0.10075</v>
       </c>
     </row>
     <row r="155" spans="1:38">
@@ -18438,16 +18438,16 @@
         <v>63</v>
       </c>
       <c r="C155">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D155">
-        <v>0.4884210526315789</v>
+        <v>0.48</v>
       </c>
       <c r="E155">
         <v>0.09974278365247213</v>
       </c>
       <c r="F155">
-        <v>0.01175667105712474</v>
+        <v>0.01902531830821016</v>
       </c>
       <c r="G155">
         <v>0</v>
@@ -18468,7 +18468,7 @@
         <v>0</v>
       </c>
       <c r="M155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N155">
         <v>0</v>
@@ -18477,13 +18477,13 @@
         <v>0</v>
       </c>
       <c r="P155">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q155">
         <v>0</v>
       </c>
       <c r="R155">
-        <v>0.04095124375016729</v>
+        <v>0.03570336066849773</v>
       </c>
       <c r="S155">
         <v>0.2466666666666667</v>
@@ -18492,13 +18492,13 @@
         <v>0.02466666666666667</v>
       </c>
       <c r="U155">
-        <v>0.1747311827956989</v>
+        <v>-1</v>
       </c>
       <c r="V155">
         <v>-1</v>
       </c>
       <c r="W155">
-        <v>0.1476014760147601</v>
+        <v>0.2306273062730627</v>
       </c>
       <c r="X155">
         <v>1</v>
@@ -18531,19 +18531,19 @@
         <v>0</v>
       </c>
       <c r="AH155">
-        <v>0.7254901960784313</v>
+        <v>1</v>
       </c>
       <c r="AI155">
-        <v>0.02920962199312714</v>
+        <v>0.05154639175257732</v>
       </c>
       <c r="AJ155">
-        <v>0.02145716293158488</v>
+        <v>0.01772548242174403</v>
       </c>
       <c r="AK155">
-        <v>0.02641253108428395</v>
+        <v>0.02647083689241703</v>
       </c>
       <c r="AL155">
-        <v>0.10075</v>
+        <v>0.06464</v>
       </c>
     </row>
     <row r="156" spans="1:38">
@@ -18554,16 +18554,16 @@
         <v>63</v>
       </c>
       <c r="C156">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D156">
-        <v>0.48</v>
+        <v>0.4842105263157895</v>
       </c>
       <c r="E156">
-        <v>0.09974278365247213</v>
+        <v>0.04829951414689911</v>
       </c>
       <c r="F156">
-        <v>0.01902531830821016</v>
+        <v>0.009707790623932875</v>
       </c>
       <c r="G156">
         <v>0</v>
@@ -18599,7 +18599,7 @@
         <v>0</v>
       </c>
       <c r="R156">
-        <v>0.03570336066849773</v>
+        <v>0.08015974360900373</v>
       </c>
       <c r="S156">
         <v>0.2466666666666667</v>
@@ -18647,19 +18647,19 @@
         <v>0</v>
       </c>
       <c r="AH156">
-        <v>1</v>
+        <v>0.8823529411764706</v>
       </c>
       <c r="AI156">
-        <v>0.05154639175257732</v>
+        <v>0.009621993127147767</v>
       </c>
       <c r="AJ156">
-        <v>0.01772548242174403</v>
+        <v>0.01290928226373068</v>
       </c>
       <c r="AK156">
-        <v>0.02647083689241703</v>
+        <v>0.01454146854838944</v>
       </c>
       <c r="AL156">
-        <v>0.06464</v>
+        <v>0.03190399999999999</v>
       </c>
     </row>
     <row r="157" spans="1:38">
@@ -18670,16 +18670,16 @@
         <v>63</v>
       </c>
       <c r="C157">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D157">
-        <v>0.4842105263157895</v>
+        <v>0.4778947368421053</v>
       </c>
       <c r="E157">
-        <v>0.04829951414689911</v>
+        <v>0.09974278365247213</v>
       </c>
       <c r="F157">
-        <v>0.009707790623932875</v>
+        <v>0.005610029757549149</v>
       </c>
       <c r="G157">
         <v>0</v>
@@ -18700,7 +18700,7 @@
         <v>0</v>
       </c>
       <c r="M157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N157">
         <v>0</v>
@@ -18709,13 +18709,13 @@
         <v>0</v>
       </c>
       <c r="P157">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q157">
         <v>0</v>
       </c>
       <c r="R157">
-        <v>0.08015974360900373</v>
+        <v>0.02915326154075105</v>
       </c>
       <c r="S157">
         <v>0.2466666666666667</v>
@@ -18724,13 +18724,13 @@
         <v>0.02466666666666667</v>
       </c>
       <c r="U157">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="V157">
-        <v>-1</v>
+        <v>0.4918032786885246</v>
       </c>
       <c r="W157">
-        <v>0.2306273062730627</v>
+        <v>0.1254612546125461</v>
       </c>
       <c r="X157">
         <v>1</v>
@@ -18763,19 +18763,19 @@
         <v>0</v>
       </c>
       <c r="AH157">
-        <v>0.8823529411764706</v>
+        <v>-1</v>
       </c>
       <c r="AI157">
-        <v>0.009621993127147767</v>
+        <v>0.0004639175257731959</v>
       </c>
       <c r="AJ157">
-        <v>0.01290928226373068</v>
+        <v>0.002928494587605572</v>
       </c>
       <c r="AK157">
-        <v>0.01454146854838944</v>
+        <v>0.003007122054463455</v>
       </c>
       <c r="AL157">
-        <v>0.03190399999999999</v>
+        <v>0.0004632352941176471</v>
       </c>
     </row>
     <row r="158" spans="1:38">
@@ -18786,13 +18786,13 @@
         <v>63</v>
       </c>
       <c r="C158">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D158">
-        <v>0.4778947368421053</v>
+        <v>0.4863157894736842</v>
       </c>
       <c r="E158">
-        <v>0.09974278365247213</v>
+        <v>0.04829951414689911</v>
       </c>
       <c r="F158">
         <v>0.005610029757549149</v>
@@ -18831,7 +18831,7 @@
         <v>0</v>
       </c>
       <c r="R158">
-        <v>0.02915326154075105</v>
+        <v>0.06453085636446647</v>
       </c>
       <c r="S158">
         <v>0.2466666666666667</v>
@@ -18840,13 +18840,13 @@
         <v>0.02466666666666667</v>
       </c>
       <c r="U158">
-        <v>0</v>
+        <v>0.05376344086021505</v>
       </c>
       <c r="V158">
-        <v>0.4918032786885246</v>
+        <v>-1</v>
       </c>
       <c r="W158">
-        <v>0.1254612546125461</v>
+        <v>0.04428044280442804</v>
       </c>
       <c r="X158">
         <v>1</v>
@@ -18879,134 +18879,18 @@
         <v>0</v>
       </c>
       <c r="AH158">
-        <v>-1</v>
+        <v>0.5490196078431373</v>
       </c>
       <c r="AI158">
-        <v>0.0004639175257731959</v>
+        <v>0.8917525773195876</v>
       </c>
       <c r="AJ158">
-        <v>0.002928494587605572</v>
+        <v>0.002915958473392824</v>
       </c>
       <c r="AK158">
-        <v>0.003007122054463455</v>
+        <v>0.1542194455700704</v>
       </c>
       <c r="AL158">
-        <v>0.0004632352941176471</v>
-      </c>
-    </row>
-    <row r="159" spans="1:38">
-      <c r="A159" s="1">
-        <v>157</v>
-      </c>
-      <c r="B159" t="s">
-        <v>63</v>
-      </c>
-      <c r="C159">
-        <v>9</v>
-      </c>
-      <c r="D159">
-        <v>0.4863157894736842</v>
-      </c>
-      <c r="E159">
-        <v>0.04829951414689911</v>
-      </c>
-      <c r="F159">
-        <v>0.005610029757549149</v>
-      </c>
-      <c r="G159">
-        <v>0</v>
-      </c>
-      <c r="H159">
-        <v>0</v>
-      </c>
-      <c r="I159">
-        <v>1</v>
-      </c>
-      <c r="J159">
-        <v>0</v>
-      </c>
-      <c r="K159">
-        <v>0</v>
-      </c>
-      <c r="L159">
-        <v>0</v>
-      </c>
-      <c r="M159">
-        <v>1</v>
-      </c>
-      <c r="N159">
-        <v>0</v>
-      </c>
-      <c r="O159">
-        <v>0</v>
-      </c>
-      <c r="P159">
-        <v>0</v>
-      </c>
-      <c r="Q159">
-        <v>0</v>
-      </c>
-      <c r="R159">
-        <v>0.06453085636446647</v>
-      </c>
-      <c r="S159">
-        <v>0.2466666666666667</v>
-      </c>
-      <c r="T159">
-        <v>0.02466666666666667</v>
-      </c>
-      <c r="U159">
-        <v>0.05376344086021505</v>
-      </c>
-      <c r="V159">
-        <v>-1</v>
-      </c>
-      <c r="W159">
-        <v>0.04428044280442804</v>
-      </c>
-      <c r="X159">
-        <v>1</v>
-      </c>
-      <c r="Y159">
-        <v>0</v>
-      </c>
-      <c r="Z159">
-        <v>0</v>
-      </c>
-      <c r="AA159">
-        <v>0</v>
-      </c>
-      <c r="AB159">
-        <v>0</v>
-      </c>
-      <c r="AC159">
-        <v>1</v>
-      </c>
-      <c r="AD159">
-        <v>1</v>
-      </c>
-      <c r="AE159">
-        <v>1</v>
-      </c>
-      <c r="AF159">
-        <v>0</v>
-      </c>
-      <c r="AG159">
-        <v>0</v>
-      </c>
-      <c r="AH159">
-        <v>0.5490196078431373</v>
-      </c>
-      <c r="AI159">
-        <v>0.8917525773195876</v>
-      </c>
-      <c r="AJ159">
-        <v>0.002915958473392824</v>
-      </c>
-      <c r="AK159">
-        <v>0.1542194455700704</v>
-      </c>
-      <c r="AL159">
         <v>2.162508333333333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed a few errors in the dataset
</commit_message>
<xml_diff>
--- a/Datasets/Reduced_version-normalized.xlsx
+++ b/Datasets/Reduced_version-normalized.xlsx
@@ -7659,7 +7659,7 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>0.02561100541489829</v>
+        <v>0.6146641299575589</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -7775,7 +7775,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>0.02561100541489829</v>
+        <v>0.6146641299575589</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -7891,7 +7891,7 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>0.02561100541489829</v>
+        <v>0.6146641299575589</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -8007,7 +8007,7 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>0.02561100541489829</v>
+        <v>0.6146641299575589</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -8123,7 +8123,7 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0.02561100541489829</v>
+        <v>0.6146641299575589</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -8239,7 +8239,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0.01912288404312406</v>
+        <v>0.4589492170349773</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -8355,7 +8355,7 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>0.01912288404312406</v>
+        <v>0.4589492170349773</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -8471,7 +8471,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>0.01912288404312406</v>
+        <v>0.4589492170349773</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -8587,7 +8587,7 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>0.01912288404312406</v>
+        <v>0.4589492170349773</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -8703,7 +8703,7 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>0.01912288404312406</v>
+        <v>0.4589492170349773</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -8819,7 +8819,7 @@
         <v>0</v>
       </c>
       <c r="F72">
-        <v>0.01912288404312406</v>
+        <v>0.4589492170349773</v>
       </c>
       <c r="G72">
         <v>0</v>

</xml_diff>